<commit_message>
拆分 mdf 为 rule 和widget
</commit_message>
<xml_diff>
--- a/storage/script/seeds/100.action.xlsx
+++ b/storage/script/seeds/100.action.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samw/project/nbkit/mdf/storage/seeds/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samw/project/nbkit/mdf/storage/script/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EA4C32-9372-984F-8A5A-AB7B5F749D77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BABAB4-7062-1848-8A77-41C63B33F562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="960" windowWidth="28240" windowHeight="17040" activeTab="1" xr2:uid="{DEC9D3BA-B19C-754D-8160-C0D8B420BE18}"/>
+    <workbookView xWindow="2120" yWindow="4420" windowWidth="28240" windowHeight="17040" activeTab="1" xr2:uid="{DEC9D3BA-B19C-754D-8160-C0D8B420BE18}"/>
   </bookViews>
   <sheets>
     <sheet name="Command" sheetId="2" r:id="rId1"/>
@@ -434,7 +434,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -722,7 +722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -748,12 +748,12 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="K11" sqref="A1:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" customWidth="1"/>
   </cols>

</xml_diff>